<commit_message>
refactor: reformat and solve warnings in some files before pulling
</commit_message>
<xml_diff>
--- a/Documentation/CosineSimilarity/Record.xlsx
+++ b/Documentation/CosineSimilarity/Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\embeders-semantic-analysis\Documentation\CosineSimilarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B223706-6F3F-4F71-B8E4-4A592831373B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5F4FF2-6562-4321-96F0-F2C78DB267A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="words vs words" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +540,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,14 +562,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +660,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-CA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3725,7 +3732,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-CA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4485,7 +4492,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-CA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5365,7 +5372,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-CA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11384,15 +11391,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>145676</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>156136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>115794</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142688</xdr:rowOff>
+      <xdr:colOff>183030</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11456,15 +11463,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>250265</xdr:colOff>
+      <xdr:colOff>459442</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>178548</xdr:rowOff>
+      <xdr:rowOff>171077</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>220383</xdr:colOff>
+      <xdr:colOff>429560</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>53042</xdr:rowOff>
+      <xdr:rowOff>45571</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11847,8 +11854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AA2988-5AAB-4458-847B-F75AA408FACB}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -11859,14 +11866,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" t="s">
@@ -12046,14 +12053,14 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
@@ -12213,19 +12220,19 @@
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11">
       <c r="B38" t="s">
@@ -12624,8 +12631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B395E1AC-FE3E-4EA2-ADDC-088EB33C8183}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -12636,14 +12643,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" t="s">
@@ -12875,26 +12882,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49FE91F-C29C-49F4-8576-5D811DA982A1}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="V88" sqref="V88"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="59.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.58203125" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" customWidth="1"/>
+    <col min="6" max="6" width="10.9140625" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" t="s">
@@ -13314,14 +13322,14 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" t="s">
@@ -13661,24 +13669,24 @@
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
     </row>
     <row r="48" spans="1:16">
       <c r="B48" t="s">
@@ -14539,24 +14547,24 @@
       </c>
     </row>
     <row r="70" spans="1:16">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
     </row>
     <row r="71" spans="1:16">
       <c r="B71" t="s">
@@ -15609,8 +15617,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A47:P47"/>
     <mergeCell ref="A70:P70"/>
+    <mergeCell ref="A47:M47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
refactor: refactor json helper, OpenAiTextGenerationServiceTests to avoid warnings and add tests for json helper
</commit_message>
<xml_diff>
--- a/Documentation/CosineSimilarity/Record.xlsx
+++ b/Documentation/CosineSimilarity/Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\embeders-semantic-analysis\Documentation\CosineSimilarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6DFE3C-8E30-43F2-8E97-958C5BA8D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29927FBE-69B8-4566-910E-E09F40AE2ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="3" activeTab="5" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="words vs words (3-small)" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>PESTLE vs word list 1 (small-3)</a:t>
+              <a:t>PESTLE vs word list 1 (3-small)</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
@@ -2900,7 +2900,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Words vs movies dataset</a:t>
+              <a:t>Words vs Movies dataset (ada-002)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3680,7 +3680,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> vs Lyrics dataset</a:t>
+              <a:t> vs Lyrics dataset (ada-002)</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -4457,7 +4457,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Words vs Books Dataset </a:t>
+              <a:t>Words vs Books Dataset (ada-002) </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5305,7 +5305,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>PESTLE vs word list 2 (small-3)</a:t>
+              <a:t>PESTLE vs word list 2 (3-small)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6081,7 +6081,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>words vs words (AI/ML)</a:t>
+              <a:t>words vs words (AI/ML) (3-small)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7599,7 +7599,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Words vs Books Dataset</a:t>
+              <a:t>Words vs Books Dataset (3-small)</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
@@ -8472,11 +8472,19 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> movies dataset</a:t>
+              <a:t> Movies dataset (3-small)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31685547250469254"/>
+          <c:y val="2.4691358024691357E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9248,7 +9256,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Words vs Lyrics Dataset</a:t>
+              <a:t>Words vs Lyrics Dataset (3-small)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -10028,7 +10036,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> (AI/ML)</a:t>
+              <a:t> (AI/ML) (ada-002)</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -20033,8 +20041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AA2988-5AAB-4458-847B-F75AA408FACB}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" topLeftCell="F37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -20840,7 +20848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B395E1AC-FE3E-4EA2-ADDC-088EB33C8183}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G12"/>
     </sheetView>
   </sheetViews>
@@ -21125,8 +21133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49FE91F-C29C-49F4-8576-5D811DA982A1}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView topLeftCell="F24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -21715,8 +21723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7807ADC6-4E54-4CA3-8A92-E6A4521869DA}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -22279,7 +22287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FC4377-C564-4CEE-B9B5-EACA486A658F}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -22550,8 +22558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD2A136-EED6-456E-AC4A-B8351DEBC004}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView topLeftCell="D43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>

<commit_message>
chore: add README.md files for the introduction and documentation
</commit_message>
<xml_diff>
--- a/Documentation/CosineSimilarity/Record.xlsx
+++ b/Documentation/CosineSimilarity/Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\embeders-semantic-analysis\Documentation\CosineSimilarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29927FBE-69B8-4566-910E-E09F40AE2ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C246A86-A7CF-41AD-8891-1F848AAA1989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="3" activeTab="5" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="words vs words (3-small)" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="94">
   <si>
     <t>political</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>trends</t>
-  </si>
-  <si>
-    <t>policy</t>
   </si>
   <si>
     <t>spending</t>
@@ -602,28 +599,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$3:$A$9</c:f>
+              <c:f>'words vs words (3-small)'!$A$3:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>trends</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>policy</c:v>
+                  <c:v>spending</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>spending</c:v>
+                  <c:v>trade tariffs</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>trade tariffs</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>renewable energy</c:v>
+                  <c:v>intellectual property</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>intellectual property</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>cultural values</c:v>
                 </c:pt>
               </c:strCache>
@@ -631,29 +625,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$B$3:$B$9</c:f>
+              <c:f>'words vs words (3-small)'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.35357917603761901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56120943234938203</c:v>
+                  <c:v>0.34720107847301002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34720107847301002</c:v>
+                  <c:v>0.27124844476157201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27124844476157201</c:v>
+                  <c:v>0.22714961371607501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22714961371607501</c:v>
+                  <c:v>0.35658725609020703</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35658725609020703</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.32879258611676099</c:v>
                 </c:pt>
               </c:numCache>
@@ -691,28 +682,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$3:$A$9</c:f>
+              <c:f>'words vs words (3-small)'!$A$3:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>trends</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>policy</c:v>
+                  <c:v>spending</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>spending</c:v>
+                  <c:v>trade tariffs</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>trade tariffs</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>renewable energy</c:v>
+                  <c:v>intellectual property</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>intellectual property</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>cultural values</c:v>
                 </c:pt>
               </c:strCache>
@@ -720,29 +708,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$C$3:$C$9</c:f>
+              <c:f>'words vs words (3-small)'!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.31135806241671199</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42382767995773701</c:v>
+                  <c:v>0.34798632531266599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34798632531266599</c:v>
+                  <c:v>0.27608937890030999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27608937890030999</c:v>
+                  <c:v>0.26689422251161499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26689422251161499</c:v>
+                  <c:v>0.29002094739645001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29002094739645001</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.265623384254565</c:v>
                 </c:pt>
               </c:numCache>
@@ -780,28 +765,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$3:$A$9</c:f>
+              <c:f>'words vs words (3-small)'!$A$3:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>trends</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>policy</c:v>
+                  <c:v>spending</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>spending</c:v>
+                  <c:v>trade tariffs</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>trade tariffs</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>renewable energy</c:v>
+                  <c:v>intellectual property</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>intellectual property</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>cultural values</c:v>
                 </c:pt>
               </c:strCache>
@@ -809,29 +791,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$D$3:$D$9</c:f>
+              <c:f>'words vs words (3-small)'!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.324688233518096</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.312508084219914</c:v>
+                  <c:v>0.19674494261196701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19674494261196701</c:v>
+                  <c:v>0.127178157464862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.127178157464862</c:v>
+                  <c:v>0.129120518233929</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.129120518233929</c:v>
+                  <c:v>0.161335530416201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.161335530416201</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.30731413177980199</c:v>
                 </c:pt>
               </c:numCache>
@@ -869,28 +848,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$3:$A$9</c:f>
+              <c:f>'words vs words (3-small)'!$A$3:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>trends</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>policy</c:v>
+                  <c:v>spending</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>spending</c:v>
+                  <c:v>trade tariffs</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>trade tariffs</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>renewable energy</c:v>
+                  <c:v>intellectual property</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>intellectual property</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>cultural values</c:v>
                 </c:pt>
               </c:strCache>
@@ -898,29 +874,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$E$3:$E$9</c:f>
+              <c:f>'words vs words (3-small)'!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.38502513926780702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28529207685146601</c:v>
+                  <c:v>0.21542177382073199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21542177382073199</c:v>
+                  <c:v>0.237368171461112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.237368171461112</c:v>
+                  <c:v>0.28417435670490199</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28417435670490199</c:v>
+                  <c:v>0.35120772020741498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35120772020741498</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.20886437523997101</c:v>
                 </c:pt>
               </c:numCache>
@@ -958,28 +931,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$3:$A$9</c:f>
+              <c:f>'words vs words (3-small)'!$A$3:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>trends</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>policy</c:v>
+                  <c:v>spending</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>spending</c:v>
+                  <c:v>trade tariffs</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>trade tariffs</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>renewable energy</c:v>
+                  <c:v>intellectual property</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>intellectual property</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>cultural values</c:v>
                 </c:pt>
               </c:strCache>
@@ -987,29 +957,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$F$3:$F$9</c:f>
+              <c:f>'words vs words (3-small)'!$F$3:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.21774503125623901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.533554787564963</c:v>
+                  <c:v>0.24931420147644701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24931420147644701</c:v>
+                  <c:v>0.224187535114899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.224187535114899</c:v>
+                  <c:v>0.1235979706001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1235979706001</c:v>
+                  <c:v>0.34047408104798299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34047408104798299</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.21574597067858001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1047,28 +1014,25 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$3:$A$9</c:f>
+              <c:f>'words vs words (3-small)'!$A$3:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>trends</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>policy</c:v>
+                  <c:v>spending</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>spending</c:v>
+                  <c:v>trade tariffs</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>trade tariffs</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>renewable energy</c:v>
+                  <c:v>intellectual property</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>intellectual property</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>cultural values</c:v>
                 </c:pt>
               </c:strCache>
@@ -1076,29 +1040,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$G$3:$G$9</c:f>
+              <c:f>'words vs words (3-small)'!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.300567374330591</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.347330687403196</c:v>
+                  <c:v>0.306326269415646</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.306326269415646</c:v>
+                  <c:v>0.175654208294037</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.175654208294037</c:v>
+                  <c:v>0.33956568911682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33956568911682</c:v>
+                  <c:v>0.255053837230312</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.255053837230312</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0.30092749659807799</c:v>
                 </c:pt>
               </c:numCache>
@@ -5351,7 +5312,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$B$20</c:f>
+              <c:f>'words vs words (3-small)'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5372,7 +5333,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$21:$A$26</c:f>
+              <c:f>'words vs words (3-small)'!$A$20:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5398,7 +5359,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$B$21:$B$26</c:f>
+              <c:f>'words vs words (3-small)'!$B$20:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5434,7 +5395,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$C$20</c:f>
+              <c:f>'words vs words (3-small)'!$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5455,7 +5416,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$21:$A$26</c:f>
+              <c:f>'words vs words (3-small)'!$A$20:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5481,7 +5442,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$C$21:$C$26</c:f>
+              <c:f>'words vs words (3-small)'!$C$20:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5517,7 +5478,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$D$20</c:f>
+              <c:f>'words vs words (3-small)'!$D$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5538,7 +5499,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$21:$A$26</c:f>
+              <c:f>'words vs words (3-small)'!$A$20:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5564,7 +5525,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$D$21:$D$26</c:f>
+              <c:f>'words vs words (3-small)'!$D$20:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5600,7 +5561,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$E$20</c:f>
+              <c:f>'words vs words (3-small)'!$E$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5621,7 +5582,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$21:$A$26</c:f>
+              <c:f>'words vs words (3-small)'!$A$20:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5647,7 +5608,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$E$21:$E$26</c:f>
+              <c:f>'words vs words (3-small)'!$E$20:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5683,7 +5644,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$F$20</c:f>
+              <c:f>'words vs words (3-small)'!$F$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5704,7 +5665,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$21:$A$26</c:f>
+              <c:f>'words vs words (3-small)'!$A$20:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5730,7 +5691,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$F$21:$F$26</c:f>
+              <c:f>'words vs words (3-small)'!$F$20:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5766,7 +5727,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$G$20</c:f>
+              <c:f>'words vs words (3-small)'!$G$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5787,7 +5748,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$21:$A$26</c:f>
+              <c:f>'words vs words (3-small)'!$A$20:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5813,7 +5774,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$G$21:$G$26</c:f>
+              <c:f>'words vs words (3-small)'!$G$20:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6127,7 +6088,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$B$38</c:f>
+              <c:f>'words vs words (3-small)'!$B$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6148,7 +6109,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$39:$A$44</c:f>
+              <c:f>'words vs words (3-small)'!$A$38:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6174,7 +6135,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$B$39:$B$44</c:f>
+              <c:f>'words vs words (3-small)'!$B$38:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6210,7 +6171,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$C$38</c:f>
+              <c:f>'words vs words (3-small)'!$C$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6231,7 +6192,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$39:$A$44</c:f>
+              <c:f>'words vs words (3-small)'!$A$38:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6257,7 +6218,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$C$39:$C$44</c:f>
+              <c:f>'words vs words (3-small)'!$C$38:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6293,7 +6254,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$D$38</c:f>
+              <c:f>'words vs words (3-small)'!$D$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6314,7 +6275,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$39:$A$44</c:f>
+              <c:f>'words vs words (3-small)'!$A$38:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6340,7 +6301,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$D$39:$D$44</c:f>
+              <c:f>'words vs words (3-small)'!$D$38:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6376,7 +6337,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$E$38</c:f>
+              <c:f>'words vs words (3-small)'!$E$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6397,7 +6358,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$39:$A$44</c:f>
+              <c:f>'words vs words (3-small)'!$A$38:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6423,7 +6384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$E$39:$E$44</c:f>
+              <c:f>'words vs words (3-small)'!$E$38:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6459,7 +6420,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$F$38</c:f>
+              <c:f>'words vs words (3-small)'!$F$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6480,7 +6441,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$39:$A$44</c:f>
+              <c:f>'words vs words (3-small)'!$A$38:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6506,7 +6467,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$F$39:$F$44</c:f>
+              <c:f>'words vs words (3-small)'!$F$38:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6542,7 +6503,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$G$38</c:f>
+              <c:f>'words vs words (3-small)'!$G$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6563,7 +6524,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'words vs words (3-small)'!$A$39:$A$44</c:f>
+              <c:f>'words vs words (3-small)'!$A$38:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6589,7 +6550,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'words vs words (3-small)'!$G$39:$G$44</c:f>
+              <c:f>'words vs words (3-small)'!$G$38:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -19200,7 +19161,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>227958</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>107587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19230,13 +19191,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>497587</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>15588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>346364</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>95770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19266,13 +19227,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>124732</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>159203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>61232</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>156481</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -20039,10 +20000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AA2988-5AAB-4458-847B-F75AA408FACB}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -20055,7 +20016,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -20077,10 +20038,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -20111,22 +20072,22 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>0.56120943234938203</v>
+        <v>0.34720107847301002</v>
       </c>
       <c r="C4">
-        <v>0.42382767995773701</v>
+        <v>0.34798632531266599</v>
       </c>
       <c r="D4">
-        <v>0.312508084219914</v>
+        <v>0.19674494261196701</v>
       </c>
       <c r="E4">
-        <v>0.28529207685146601</v>
+        <v>0.21542177382073199</v>
       </c>
       <c r="F4">
-        <v>0.533554787564963</v>
+        <v>0.24931420147644701</v>
       </c>
       <c r="G4">
-        <v>0.347330687403196</v>
+        <v>0.306326269415646</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -20134,22 +20095,22 @@
         <v>41</v>
       </c>
       <c r="B5">
-        <v>0.34720107847301002</v>
+        <v>0.27124844476157201</v>
       </c>
       <c r="C5">
-        <v>0.34798632531266599</v>
+        <v>0.27608937890030999</v>
       </c>
       <c r="D5">
-        <v>0.19674494261196701</v>
+        <v>0.127178157464862</v>
       </c>
       <c r="E5">
-        <v>0.21542177382073199</v>
+        <v>0.237368171461112</v>
       </c>
       <c r="F5">
-        <v>0.24931420147644701</v>
+        <v>0.224187535114899</v>
       </c>
       <c r="G5">
-        <v>0.306326269415646</v>
+        <v>0.175654208294037</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -20157,22 +20118,22 @@
         <v>42</v>
       </c>
       <c r="B6">
-        <v>0.27124844476157201</v>
+        <v>0.22714961371607501</v>
       </c>
       <c r="C6">
-        <v>0.27608937890030999</v>
+        <v>0.26689422251161499</v>
       </c>
       <c r="D6">
-        <v>0.127178157464862</v>
+        <v>0.129120518233929</v>
       </c>
       <c r="E6">
-        <v>0.237368171461112</v>
+        <v>0.28417435670490199</v>
       </c>
       <c r="F6">
-        <v>0.224187535114899</v>
+        <v>0.1235979706001</v>
       </c>
       <c r="G6">
-        <v>0.175654208294037</v>
+        <v>0.33956568911682</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -20180,22 +20141,22 @@
         <v>43</v>
       </c>
       <c r="B7">
-        <v>0.22714961371607501</v>
+        <v>0.35658725609020703</v>
       </c>
       <c r="C7">
-        <v>0.26689422251161499</v>
+        <v>0.29002094739645001</v>
       </c>
       <c r="D7">
-        <v>0.129120518233929</v>
+        <v>0.161335530416201</v>
       </c>
       <c r="E7">
-        <v>0.28417435670490199</v>
+        <v>0.35120772020741498</v>
       </c>
       <c r="F7">
-        <v>0.1235979706001</v>
+        <v>0.34047408104798299</v>
       </c>
       <c r="G7">
-        <v>0.33956568911682</v>
+        <v>0.255053837230312</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -20203,75 +20164,75 @@
         <v>44</v>
       </c>
       <c r="B8">
-        <v>0.35658725609020703</v>
+        <v>0.32879258611676099</v>
       </c>
       <c r="C8">
-        <v>0.29002094739645001</v>
+        <v>0.265623384254565</v>
       </c>
       <c r="D8">
-        <v>0.161335530416201</v>
+        <v>0.30731413177980199</v>
       </c>
       <c r="E8">
-        <v>0.35120772020741498</v>
+        <v>0.20886437523997101</v>
       </c>
       <c r="F8">
-        <v>0.34047408104798299</v>
+        <v>0.21574597067858001</v>
       </c>
       <c r="G8">
-        <v>0.255053837230312</v>
+        <v>0.30092749659807799</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9">
-        <v>0.32879258611676099</v>
-      </c>
-      <c r="C9">
-        <v>0.265623384254565</v>
-      </c>
-      <c r="D9">
-        <v>0.30731413177980199</v>
-      </c>
-      <c r="E9">
-        <v>0.20886437523997101</v>
-      </c>
-      <c r="F9">
-        <v>0.21574597067858001</v>
-      </c>
-      <c r="G9">
-        <v>0.30092749659807799</v>
-      </c>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" t="s">
-        <v>94</v>
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20">
+        <v>0.34468539924810199</v>
+      </c>
+      <c r="C20">
+        <v>0.33816511431690599</v>
+      </c>
+      <c r="D20">
+        <v>0.22872785405784901</v>
+      </c>
+      <c r="E20">
+        <v>0.28743734591749598</v>
+      </c>
+      <c r="F20">
+        <v>0.357351756516888</v>
+      </c>
+      <c r="G20">
+        <v>0.361879444053197</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -20279,22 +20240,22 @@
         <v>47</v>
       </c>
       <c r="B21">
-        <v>0.34468539924810199</v>
+        <v>0.34105290878137801</v>
       </c>
       <c r="C21">
-        <v>0.33816511431690599</v>
+        <v>0.26741089309209598</v>
       </c>
       <c r="D21">
-        <v>0.22872785405784901</v>
+        <v>0.25527028797747398</v>
       </c>
       <c r="E21">
-        <v>0.28743734591749598</v>
+        <v>0.29023641488413998</v>
       </c>
       <c r="F21">
-        <v>0.357351756516888</v>
+        <v>0.222913413988239</v>
       </c>
       <c r="G21">
-        <v>0.361879444053197</v>
+        <v>0.23181266624250399</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -20302,22 +20263,22 @@
         <v>48</v>
       </c>
       <c r="B22">
-        <v>0.34105290878137801</v>
+        <v>0.40723198971739299</v>
       </c>
       <c r="C22">
-        <v>0.26741089309209598</v>
+        <v>0.34638403856303301</v>
       </c>
       <c r="D22">
-        <v>0.25527028797747398</v>
+        <v>0.25292503628881602</v>
       </c>
       <c r="E22">
-        <v>0.29023641488413998</v>
+        <v>0.31962759287943598</v>
       </c>
       <c r="F22">
-        <v>0.222913413988239</v>
+        <v>0.28224617470305802</v>
       </c>
       <c r="G22">
-        <v>0.23181266624250399</v>
+        <v>0.34098216542160398</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -20325,22 +20286,22 @@
         <v>49</v>
       </c>
       <c r="B23">
-        <v>0.40723198971739299</v>
+        <v>0.27148462680298402</v>
       </c>
       <c r="C23">
-        <v>0.34638403856303301</v>
+        <v>0.32391023074272901</v>
       </c>
       <c r="D23">
-        <v>0.25292503628881602</v>
+        <v>0.20224431508610799</v>
       </c>
       <c r="E23">
-        <v>0.31962759287943598</v>
+        <v>0.247391618462761</v>
       </c>
       <c r="F23">
-        <v>0.28224617470305802</v>
+        <v>0.367773103678041</v>
       </c>
       <c r="G23">
-        <v>0.34098216542160398</v>
+        <v>0.27988656761356701</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -20348,138 +20309,150 @@
         <v>50</v>
       </c>
       <c r="B24">
-        <v>0.27148462680298402</v>
+        <v>0.38817657693851498</v>
       </c>
       <c r="C24">
-        <v>0.32391023074272901</v>
+        <v>0.37899641998323202</v>
       </c>
       <c r="D24">
-        <v>0.20224431508610799</v>
+        <v>0.27473369741699399</v>
       </c>
       <c r="E24">
-        <v>0.247391618462761</v>
+        <v>0.29090411747751299</v>
       </c>
       <c r="F24">
-        <v>0.367773103678041</v>
+        <v>0.20842223220093301</v>
       </c>
       <c r="G24">
-        <v>0.27988656761356701</v>
+        <v>0.35719110508929403</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B25">
-        <v>0.38817657693851498</v>
+        <v>0.32001130466665201</v>
       </c>
       <c r="C25">
-        <v>0.37899641998323202</v>
+        <v>0.29153690768142798</v>
       </c>
       <c r="D25">
-        <v>0.27473369741699399</v>
+        <v>0.23470285265818699</v>
       </c>
       <c r="E25">
-        <v>0.29090411747751299</v>
+        <v>0.23015936577718099</v>
       </c>
       <c r="F25">
-        <v>0.20842223220093301</v>
+        <v>0.37102480442409902</v>
       </c>
       <c r="G25">
-        <v>0.35719110508929403</v>
+        <v>0.314021178038078</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B26">
-        <v>0.32001130466665201</v>
+        <v>0.35038281471919702</v>
       </c>
       <c r="C26">
-        <v>0.29153690768142798</v>
+        <v>0.42126269092983598</v>
       </c>
       <c r="D26">
-        <v>0.23470285265818699</v>
+        <v>0.227130336974803</v>
       </c>
       <c r="E26">
-        <v>0.23015936577718099</v>
+        <v>0.26510556188714901</v>
       </c>
       <c r="F26">
-        <v>0.37102480442409902</v>
+        <v>0.30819492751069399</v>
       </c>
       <c r="G26">
-        <v>0.314021178038078</v>
+        <v>0.38009059331210499</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27">
-        <v>0.35038281471919702</v>
-      </c>
-      <c r="C27">
-        <v>0.42126269092983598</v>
-      </c>
-      <c r="D27">
-        <v>0.227130336974803</v>
-      </c>
-      <c r="E27">
-        <v>0.26510556188714901</v>
-      </c>
-      <c r="F27">
-        <v>0.30819492751069399</v>
-      </c>
-      <c r="G27">
-        <v>0.38009059331210499</v>
-      </c>
+    <row r="36" spans="1:11">
+      <c r="A36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" t="s">
+        <v>59</v>
+      </c>
+      <c r="I37" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" t="s">
+        <v>61</v>
+      </c>
+      <c r="K37" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="B38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" t="s">
-        <v>59</v>
-      </c>
-      <c r="H38" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" t="s">
-        <v>61</v>
-      </c>
-      <c r="J38" t="s">
-        <v>62</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="A38" t="s">
         <v>63</v>
+      </c>
+      <c r="B38">
+        <v>0.48632557504159901</v>
+      </c>
+      <c r="C38">
+        <v>0.27631132329278302</v>
+      </c>
+      <c r="D38">
+        <v>0.42509986857093701</v>
+      </c>
+      <c r="E38">
+        <v>0.39922455230404102</v>
+      </c>
+      <c r="F38">
+        <v>0.377263103928066</v>
+      </c>
+      <c r="G38">
+        <v>0.39917581785192602</v>
+      </c>
+      <c r="H38">
+        <v>0.34253541042449798</v>
+      </c>
+      <c r="I38">
+        <v>0.32086231632333301</v>
+      </c>
+      <c r="J38">
+        <v>0.33863343437123899</v>
+      </c>
+      <c r="K38">
+        <v>0.25324236494709601</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -20487,34 +20460,34 @@
         <v>64</v>
       </c>
       <c r="B39">
-        <v>0.48632557504159901</v>
+        <v>0.438552544660398</v>
       </c>
       <c r="C39">
-        <v>0.27631132329278302</v>
+        <v>0.236551164752768</v>
       </c>
       <c r="D39">
-        <v>0.42509986857093701</v>
+        <v>0.24291987588106501</v>
       </c>
       <c r="E39">
-        <v>0.39922455230404102</v>
+        <v>0.34435198885198898</v>
       </c>
       <c r="F39">
-        <v>0.377263103928066</v>
+        <v>0.29416494198927701</v>
       </c>
       <c r="G39">
-        <v>0.39917581785192602</v>
+        <v>0.37750604413087402</v>
       </c>
       <c r="H39">
-        <v>0.34253541042449798</v>
+        <v>0.28654090866833598</v>
       </c>
       <c r="I39">
-        <v>0.32086231632333301</v>
+        <v>0.27380134286838198</v>
       </c>
       <c r="J39">
-        <v>0.33863343437123899</v>
+        <v>0.32510983269760202</v>
       </c>
       <c r="K39">
-        <v>0.25324236494709601</v>
+        <v>0.197859778796909</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -20522,34 +20495,34 @@
         <v>65</v>
       </c>
       <c r="B40">
-        <v>0.438552544660398</v>
+        <v>0.35504728935131802</v>
       </c>
       <c r="C40">
-        <v>0.236551164752768</v>
+        <v>0.155578175462389</v>
       </c>
       <c r="D40">
-        <v>0.24291987588106501</v>
+        <v>0.23214185482186001</v>
       </c>
       <c r="E40">
-        <v>0.34435198885198898</v>
+        <v>0.39192462673057898</v>
       </c>
       <c r="F40">
-        <v>0.29416494198927701</v>
+        <v>0.26909333610526398</v>
       </c>
       <c r="G40">
-        <v>0.37750604413087402</v>
+        <v>0.54268860348931602</v>
       </c>
       <c r="H40">
-        <v>0.28654090866833598</v>
+        <v>0.23214934941156601</v>
       </c>
       <c r="I40">
-        <v>0.27380134286838198</v>
+        <v>0.295234833488208</v>
       </c>
       <c r="J40">
-        <v>0.32510983269760202</v>
+        <v>0.23586044210210499</v>
       </c>
       <c r="K40">
-        <v>0.197859778796909</v>
+        <v>0.106737252225512</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -20557,34 +20530,34 @@
         <v>66</v>
       </c>
       <c r="B41">
-        <v>0.35504728935131802</v>
+        <v>0.36334533383774198</v>
       </c>
       <c r="C41">
-        <v>0.155578175462389</v>
+        <v>0.26495178981018802</v>
       </c>
       <c r="D41">
-        <v>0.23214185482186001</v>
+        <v>0.23044503479970599</v>
       </c>
       <c r="E41">
-        <v>0.39192462673057898</v>
+        <v>0.29610109152156899</v>
       </c>
       <c r="F41">
-        <v>0.26909333610526398</v>
+        <v>0.36531009257546598</v>
       </c>
       <c r="G41">
-        <v>0.54268860348931602</v>
+        <v>0.36588981392226599</v>
       </c>
       <c r="H41">
-        <v>0.23214934941156601</v>
+        <v>0.333840389502575</v>
       </c>
       <c r="I41">
-        <v>0.295234833488208</v>
+        <v>0.28603318956664697</v>
       </c>
       <c r="J41">
-        <v>0.23586044210210499</v>
+        <v>0.38267857165553498</v>
       </c>
       <c r="K41">
-        <v>0.106737252225512</v>
+        <v>0.27736529616222</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -20592,34 +20565,34 @@
         <v>67</v>
       </c>
       <c r="B42">
-        <v>0.36334533383774198</v>
+        <v>0.335374243906497</v>
       </c>
       <c r="C42">
-        <v>0.26495178981018802</v>
+        <v>0.16100893917293399</v>
       </c>
       <c r="D42">
-        <v>0.23044503479970599</v>
+        <v>0.276884821651741</v>
       </c>
       <c r="E42">
-        <v>0.29610109152156899</v>
+        <v>0.25682785681043202</v>
       </c>
       <c r="F42">
-        <v>0.36531009257546598</v>
+        <v>0.209010369320835</v>
       </c>
       <c r="G42">
-        <v>0.36588981392226599</v>
+        <v>0.27716573001690198</v>
       </c>
       <c r="H42">
-        <v>0.333840389502575</v>
+        <v>0.32508122370352499</v>
       </c>
       <c r="I42">
-        <v>0.28603318956664697</v>
+        <v>0.26875371093177203</v>
       </c>
       <c r="J42">
-        <v>0.38267857165553498</v>
+        <v>0.25981706250782099</v>
       </c>
       <c r="K42">
-        <v>0.27736529616222</v>
+        <v>0.25852442771144901</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -20627,34 +20600,34 @@
         <v>68</v>
       </c>
       <c r="B43">
-        <v>0.335374243906497</v>
+        <v>0.30508797507700902</v>
       </c>
       <c r="C43">
-        <v>0.16100893917293399</v>
+        <v>0.35836226367267499</v>
       </c>
       <c r="D43">
-        <v>0.276884821651741</v>
+        <v>0.24211839910906499</v>
       </c>
       <c r="E43">
-        <v>0.25682785681043202</v>
+        <v>0.26513333305040399</v>
       </c>
       <c r="F43">
-        <v>0.209010369320835</v>
+        <v>0.19711632178157701</v>
       </c>
       <c r="G43">
-        <v>0.27716573001690198</v>
+        <v>0.30373228529516599</v>
       </c>
       <c r="H43">
-        <v>0.32508122370352499</v>
+        <v>0.226326115081014</v>
       </c>
       <c r="I43">
-        <v>0.26875371093177203</v>
+        <v>0.29754310051010802</v>
       </c>
       <c r="J43">
-        <v>0.25981706250782099</v>
+        <v>0.16994410828919901</v>
       </c>
       <c r="K43">
-        <v>0.25852442771144901</v>
+        <v>0.124500283528362</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -20662,34 +20635,34 @@
         <v>69</v>
       </c>
       <c r="B44">
-        <v>0.30508797507700902</v>
+        <v>0.21841999174225599</v>
       </c>
       <c r="C44">
-        <v>0.35836226367267499</v>
+        <v>0.184780896255759</v>
       </c>
       <c r="D44">
-        <v>0.24211839910906499</v>
+        <v>0.193936674331706</v>
       </c>
       <c r="E44">
-        <v>0.26513333305040399</v>
+        <v>0.40464901999785402</v>
       </c>
       <c r="F44">
-        <v>0.19711632178157701</v>
+        <v>0.21151754005102499</v>
       </c>
       <c r="G44">
-        <v>0.30373228529516599</v>
+        <v>0.31325204128476902</v>
       </c>
       <c r="H44">
-        <v>0.226326115081014</v>
+        <v>0.228985741644814</v>
       </c>
       <c r="I44">
-        <v>0.29754310051010802</v>
+        <v>0.27763870171417099</v>
       </c>
       <c r="J44">
-        <v>0.16994410828919901</v>
+        <v>0.21114249012192601</v>
       </c>
       <c r="K44">
-        <v>0.124500283528362</v>
+        <v>0.108270127924046</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -20697,34 +20670,34 @@
         <v>70</v>
       </c>
       <c r="B45">
-        <v>0.21841999174225599</v>
+        <v>0.31649023543798899</v>
       </c>
       <c r="C45">
-        <v>0.184780896255759</v>
+        <v>0.18759023330986299</v>
       </c>
       <c r="D45">
-        <v>0.193936674331706</v>
+        <v>0.27432029592789597</v>
       </c>
       <c r="E45">
-        <v>0.40464901999785402</v>
+        <v>0.53619104708998799</v>
       </c>
       <c r="F45">
-        <v>0.21151754005102499</v>
+        <v>0.30427229601650901</v>
       </c>
       <c r="G45">
-        <v>0.31325204128476902</v>
+        <v>0.37080940338400098</v>
       </c>
       <c r="H45">
-        <v>0.228985741644814</v>
+        <v>0.284358950653193</v>
       </c>
       <c r="I45">
-        <v>0.27763870171417099</v>
+        <v>0.21784998417476001</v>
       </c>
       <c r="J45">
-        <v>0.21114249012192601</v>
+        <v>0.23092121948605701</v>
       </c>
       <c r="K45">
-        <v>0.108270127924046</v>
+        <v>0.13329840618659899</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -20732,111 +20705,76 @@
         <v>71</v>
       </c>
       <c r="B46">
-        <v>0.31649023543798899</v>
+        <v>0.39734651482857503</v>
       </c>
       <c r="C46">
-        <v>0.18759023330986299</v>
+        <v>0.240812138244476</v>
       </c>
       <c r="D46">
-        <v>0.27432029592789597</v>
+        <v>0.39286494253889498</v>
       </c>
       <c r="E46">
-        <v>0.53619104708998799</v>
+        <v>0.38549508860301501</v>
       </c>
       <c r="F46">
-        <v>0.30427229601650901</v>
+        <v>0.42154858519347499</v>
       </c>
       <c r="G46">
-        <v>0.37080940338400098</v>
+        <v>0.45007892743394601</v>
       </c>
       <c r="H46">
-        <v>0.284358950653193</v>
+        <v>0.34332154749350402</v>
       </c>
       <c r="I46">
-        <v>0.21784998417476001</v>
+        <v>0.31875963904548499</v>
       </c>
       <c r="J46">
-        <v>0.23092121948605701</v>
+        <v>0.36147785604445998</v>
       </c>
       <c r="K46">
-        <v>0.13329840618659899</v>
+        <v>0.324184293510554</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B47">
-        <v>0.39734651482857503</v>
+        <v>0.38782704063191897</v>
       </c>
       <c r="C47">
-        <v>0.240812138244476</v>
+        <v>0.27447680832826699</v>
       </c>
       <c r="D47">
-        <v>0.39286494253889498</v>
+        <v>0.33582152342961302</v>
       </c>
       <c r="E47">
-        <v>0.38549508860301501</v>
+        <v>0.44866764455735297</v>
       </c>
       <c r="F47">
-        <v>0.42154858519347499</v>
+        <v>0.26918662155865603</v>
       </c>
       <c r="G47">
-        <v>0.45007892743394601</v>
+        <v>0.50002206974385299</v>
       </c>
       <c r="H47">
-        <v>0.34332154749350402</v>
+        <v>0.24694188442662901</v>
       </c>
       <c r="I47">
-        <v>0.31875963904548499</v>
+        <v>0.32557814056442302</v>
       </c>
       <c r="J47">
-        <v>0.36147785604445998</v>
+        <v>0.22764144275297499</v>
       </c>
       <c r="K47">
-        <v>0.324184293510554</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48">
-        <v>0.38782704063191897</v>
-      </c>
-      <c r="C48">
-        <v>0.27447680832826699</v>
-      </c>
-      <c r="D48">
-        <v>0.33582152342961302</v>
-      </c>
-      <c r="E48">
-        <v>0.44866764455735297</v>
-      </c>
-      <c r="F48">
-        <v>0.26918662155865603</v>
-      </c>
-      <c r="G48">
-        <v>0.50002206974385299</v>
-      </c>
-      <c r="H48">
-        <v>0.24694188442662901</v>
-      </c>
-      <c r="I48">
-        <v>0.32557814056442302</v>
-      </c>
-      <c r="J48">
-        <v>0.22764144275297499</v>
-      </c>
-      <c r="K48">
         <v>0.20813836661221899</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -20848,7 +20786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B395E1AC-FE3E-4EA2-ADDC-088EB33C8183}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G12"/>
     </sheetView>
   </sheetViews>
@@ -20883,10 +20821,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -21133,7 +21071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49FE91F-C29C-49F4-8576-5D811DA982A1}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="F24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
@@ -21148,7 +21086,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -21159,19 +21097,19 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -21364,7 +21302,7 @@
     <row r="17" spans="1:7" ht="14.5" thickBot="1"/>
     <row r="18" spans="1:7" ht="14.5" thickBot="1">
       <c r="A18" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -21376,19 +21314,19 @@
     <row r="19" spans="1:7" ht="14.5" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>12</v>
@@ -21535,7 +21473,7 @@
     <row r="35" spans="1:16" ht="14.5" thickBot="1"/>
     <row r="36" spans="1:16" ht="14.5" customHeight="1" thickBot="1">
       <c r="A36" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -21566,7 +21504,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38">
         <v>8.19784372826355E-2</v>
@@ -21589,7 +21527,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39">
         <v>0.117328676489949</v>
@@ -21612,7 +21550,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40">
         <v>7.3982943970032605E-2</v>
@@ -21635,7 +21573,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41">
         <v>8.4762973995164304E-2</v>
@@ -21658,7 +21596,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42">
         <v>7.5051965838065504E-2</v>
@@ -21681,7 +21619,7 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43">
         <v>0.207970151001547</v>
@@ -21723,7 +21661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7807ADC6-4E54-4CA3-8A92-E6A4521869DA}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -21740,7 +21678,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -21755,27 +21693,27 @@
     </row>
     <row r="2" spans="1:11">
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>57</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>0.82339587602148601</v>
@@ -21798,7 +21736,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>0.82365331208117898</v>
@@ -21821,7 +21759,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>0.80764662167332002</v>
@@ -21844,7 +21782,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>0.79169769193559103</v>
@@ -21867,7 +21805,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7">
         <v>0.80186954704820901</v>
@@ -21890,7 +21828,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>0.80807881600865294</v>
@@ -21925,10 +21863,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
         <v>93</v>
-      </c>
-      <c r="G19" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -21956,7 +21894,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>0.80574608567980899</v>
@@ -21979,7 +21917,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>0.80679219793801105</v>
@@ -22002,7 +21940,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23">
         <v>0.78192678856048703</v>
@@ -22025,7 +21963,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>0.79849199365861201</v>
@@ -22048,7 +21986,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>0.77180457583749296</v>
@@ -22071,7 +22009,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>0.78166536196522196</v>
@@ -22106,15 +22044,15 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
         <v>93</v>
-      </c>
-      <c r="G29" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>0.81614472297669904</v>
@@ -22137,7 +22075,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>0.80197989046470097</v>
@@ -22160,7 +22098,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>0.838523912551703</v>
@@ -22183,7 +22121,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>0.79924284916202903</v>
@@ -22206,7 +22144,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34">
         <v>0.84048348536483597</v>
@@ -22252,7 +22190,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36">
         <v>0.80470999400413701</v>
@@ -22287,7 +22225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FC4377-C564-4CEE-B9B5-EACA486A658F}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -22311,10 +22249,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -22558,8 +22496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD2A136-EED6-456E-AC4A-B8351DEBC004}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="D43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -22569,19 +22507,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>79</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -22793,7 +22731,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21">
         <v>0.72087117290077096</v>
@@ -22816,7 +22754,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22">
         <v>0.74251547139677698</v>
@@ -22839,7 +22777,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23">
         <v>0.74354518463169905</v>
@@ -22862,7 +22800,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24">
         <v>0.724596859181731</v>
@@ -22885,7 +22823,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25">
         <v>0.73229754503157196</v>
@@ -22908,7 +22846,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>0.74926914613655704</v>
@@ -22931,19 +22869,19 @@
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" t="s">
         <v>81</v>
-      </c>
-      <c r="D38" t="s">
-        <v>82</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
chore: merge and refactor
</commit_message>
<xml_diff>
--- a/Documentation/CosineSimilarity/Record.xlsx
+++ b/Documentation/CosineSimilarity/Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\embeders-semantic-analysis\Documentation\CosineSimilarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160DCBDA-1299-47CF-8126-E9CE37906E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A71884A-50D0-4567-AAA2-1B69878E4C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="4" activeTab="6" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="words vs words (ada-002)" sheetId="4" r:id="rId4"/>
     <sheet name="words vs pdfs (ada-002)" sheetId="5" r:id="rId5"/>
     <sheet name="words vs datasets (ada-002)" sheetId="7" r:id="rId6"/>
-    <sheet name="Retry" sheetId="9" r:id="rId7"/>
+    <sheet name="Final results" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5377,7 +5377,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$J$1</c:f>
+              <c:f>'Final results'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5398,7 +5398,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$2:$I$7</c:f>
+              <c:f>'Final results'!$I$2:$I$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5424,7 +5424,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$J$2:$J$7</c:f>
+              <c:f>'Final results'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5460,7 +5460,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$K$1</c:f>
+              <c:f>'Final results'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5481,7 +5481,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$2:$I$7</c:f>
+              <c:f>'Final results'!$I$2:$I$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5507,7 +5507,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$K$2:$K$7</c:f>
+              <c:f>'Final results'!$K$2:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5543,7 +5543,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$L$1</c:f>
+              <c:f>'Final results'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5564,7 +5564,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$2:$I$7</c:f>
+              <c:f>'Final results'!$I$2:$I$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5590,7 +5590,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$L$2:$L$7</c:f>
+              <c:f>'Final results'!$L$2:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5626,7 +5626,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$M$1</c:f>
+              <c:f>'Final results'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5647,7 +5647,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$2:$I$7</c:f>
+              <c:f>'Final results'!$I$2:$I$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5673,7 +5673,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$M$2:$M$7</c:f>
+              <c:f>'Final results'!$M$2:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5709,7 +5709,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$N$1</c:f>
+              <c:f>'Final results'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5730,7 +5730,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$2:$I$7</c:f>
+              <c:f>'Final results'!$I$2:$I$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5756,7 +5756,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$N$2:$N$7</c:f>
+              <c:f>'Final results'!$N$2:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5792,7 +5792,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$O$1</c:f>
+              <c:f>'Final results'!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5813,7 +5813,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$2:$I$7</c:f>
+              <c:f>'Final results'!$I$2:$I$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -5839,7 +5839,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$O$2:$O$7</c:f>
+              <c:f>'Final results'!$O$2:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6160,7 +6160,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$B$1</c:f>
+              <c:f>'Final results'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6181,7 +6181,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$2:$A$7</c:f>
+              <c:f>'Final results'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6207,7 +6207,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$B$2:$B$7</c:f>
+              <c:f>'Final results'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6243,7 +6243,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$C$1</c:f>
+              <c:f>'Final results'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6264,7 +6264,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$2:$A$7</c:f>
+              <c:f>'Final results'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6290,7 +6290,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$C$2:$C$7</c:f>
+              <c:f>'Final results'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6326,7 +6326,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$D$1</c:f>
+              <c:f>'Final results'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6347,7 +6347,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$2:$A$7</c:f>
+              <c:f>'Final results'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6373,7 +6373,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$D$2:$D$7</c:f>
+              <c:f>'Final results'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6409,7 +6409,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$E$1</c:f>
+              <c:f>'Final results'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6430,7 +6430,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$2:$A$7</c:f>
+              <c:f>'Final results'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6456,7 +6456,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$E$2:$E$7</c:f>
+              <c:f>'Final results'!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6492,7 +6492,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$F$1</c:f>
+              <c:f>'Final results'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6513,7 +6513,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$2:$A$7</c:f>
+              <c:f>'Final results'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6539,7 +6539,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$F$2:$F$7</c:f>
+              <c:f>'Final results'!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6575,7 +6575,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$G$1</c:f>
+              <c:f>'Final results'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6596,7 +6596,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$2:$A$7</c:f>
+              <c:f>'Final results'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6622,7 +6622,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$G$2:$G$7</c:f>
+              <c:f>'Final results'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6943,7 +6943,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$B$26</c:f>
+              <c:f>'Final results'!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6964,7 +6964,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$27:$A$32</c:f>
+              <c:f>'Final results'!$A$27:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -6990,7 +6990,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$B$27:$B$32</c:f>
+              <c:f>'Final results'!$B$27:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7026,7 +7026,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$C$26</c:f>
+              <c:f>'Final results'!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7047,7 +7047,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$27:$A$32</c:f>
+              <c:f>'Final results'!$A$27:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7073,7 +7073,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$C$27:$C$32</c:f>
+              <c:f>'Final results'!$C$27:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7109,7 +7109,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$D$26</c:f>
+              <c:f>'Final results'!$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7130,7 +7130,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$27:$A$32</c:f>
+              <c:f>'Final results'!$A$27:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7156,7 +7156,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$D$27:$D$32</c:f>
+              <c:f>'Final results'!$D$27:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7192,7 +7192,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$E$26</c:f>
+              <c:f>'Final results'!$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7213,7 +7213,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$27:$A$32</c:f>
+              <c:f>'Final results'!$A$27:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7239,7 +7239,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$E$27:$E$32</c:f>
+              <c:f>'Final results'!$E$27:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7275,7 +7275,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$F$26</c:f>
+              <c:f>'Final results'!$F$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7296,7 +7296,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$27:$A$32</c:f>
+              <c:f>'Final results'!$A$27:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7322,7 +7322,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$F$27:$F$32</c:f>
+              <c:f>'Final results'!$F$27:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7597,7 +7597,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Words vs Songs dataset (ada-002) </a:t>
+              <a:t>Words vs Songs dataset (3-small) </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7643,7 +7643,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$I$26</c:f>
+              <c:f>'Final results'!$I$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7664,7 +7664,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$H$27:$H$32</c:f>
+              <c:f>'Final results'!$H$27:$H$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7690,7 +7690,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$I$27:$I$32</c:f>
+              <c:f>'Final results'!$I$27:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7726,7 +7726,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$J$26</c:f>
+              <c:f>'Final results'!$J$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7747,7 +7747,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$H$27:$H$32</c:f>
+              <c:f>'Final results'!$H$27:$H$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7773,7 +7773,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$J$27:$J$32</c:f>
+              <c:f>'Final results'!$J$27:$J$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7809,7 +7809,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$K$26</c:f>
+              <c:f>'Final results'!$K$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7830,7 +7830,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$H$27:$H$32</c:f>
+              <c:f>'Final results'!$H$27:$H$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7856,7 +7856,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$K$27:$K$32</c:f>
+              <c:f>'Final results'!$K$27:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7892,7 +7892,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$L$26</c:f>
+              <c:f>'Final results'!$L$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7913,7 +7913,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$H$27:$H$32</c:f>
+              <c:f>'Final results'!$H$27:$H$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -7939,7 +7939,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$L$27:$L$32</c:f>
+              <c:f>'Final results'!$L$27:$L$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -7975,7 +7975,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$M$26</c:f>
+              <c:f>'Final results'!$M$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7996,7 +7996,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$H$27:$H$32</c:f>
+              <c:f>'Final results'!$H$27:$H$32</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8022,7 +8022,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$M$27:$M$32</c:f>
+              <c:f>'Final results'!$M$27:$M$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8343,7 +8343,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$B$50</c:f>
+              <c:f>'Final results'!$B$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8364,7 +8364,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$51:$A$56</c:f>
+              <c:f>'Final results'!$A$51:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8390,7 +8390,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$B$51:$B$56</c:f>
+              <c:f>'Final results'!$B$51:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8426,7 +8426,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$C$50</c:f>
+              <c:f>'Final results'!$C$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8447,7 +8447,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$51:$A$56</c:f>
+              <c:f>'Final results'!$A$51:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8473,7 +8473,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$C$51:$C$56</c:f>
+              <c:f>'Final results'!$C$51:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8509,7 +8509,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$D$50</c:f>
+              <c:f>'Final results'!$D$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8530,7 +8530,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$51:$A$56</c:f>
+              <c:f>'Final results'!$A$51:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8556,7 +8556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$D$51:$D$56</c:f>
+              <c:f>'Final results'!$D$51:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8592,7 +8592,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$E$50</c:f>
+              <c:f>'Final results'!$E$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8613,7 +8613,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$51:$A$56</c:f>
+              <c:f>'Final results'!$A$51:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8639,7 +8639,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$E$51:$E$56</c:f>
+              <c:f>'Final results'!$E$51:$E$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8675,7 +8675,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$F$50</c:f>
+              <c:f>'Final results'!$F$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8696,7 +8696,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$51:$A$56</c:f>
+              <c:f>'Final results'!$A$51:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8722,7 +8722,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$F$51:$F$56</c:f>
+              <c:f>'Final results'!$F$51:$F$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -8758,7 +8758,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$G$50</c:f>
+              <c:f>'Final results'!$G$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8779,7 +8779,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$51:$A$56</c:f>
+              <c:f>'Final results'!$A$51:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -8805,7 +8805,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$G$51:$G$56</c:f>
+              <c:f>'Final results'!$G$51:$G$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -9902,7 +9902,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$J$50</c:f>
+              <c:f>'Final results'!$J$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9923,7 +9923,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$51:$I$56</c:f>
+              <c:f>'Final results'!$I$51:$I$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -9949,7 +9949,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$J$51:$J$56</c:f>
+              <c:f>'Final results'!$J$51:$J$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -9985,7 +9985,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$K$50</c:f>
+              <c:f>'Final results'!$K$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10006,7 +10006,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$51:$I$56</c:f>
+              <c:f>'Final results'!$I$51:$I$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10032,7 +10032,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$K$51:$K$56</c:f>
+              <c:f>'Final results'!$K$51:$K$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10068,7 +10068,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$L$50</c:f>
+              <c:f>'Final results'!$L$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10089,7 +10089,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$51:$I$56</c:f>
+              <c:f>'Final results'!$I$51:$I$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10115,7 +10115,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$L$51:$L$56</c:f>
+              <c:f>'Final results'!$L$51:$L$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10151,7 +10151,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$M$50</c:f>
+              <c:f>'Final results'!$M$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10172,7 +10172,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$51:$I$56</c:f>
+              <c:f>'Final results'!$I$51:$I$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10198,7 +10198,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$M$51:$M$56</c:f>
+              <c:f>'Final results'!$M$51:$M$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10234,7 +10234,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$N$50</c:f>
+              <c:f>'Final results'!$N$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10255,7 +10255,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$51:$I$56</c:f>
+              <c:f>'Final results'!$I$51:$I$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10281,7 +10281,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$N$51:$N$56</c:f>
+              <c:f>'Final results'!$N$51:$N$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10317,7 +10317,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$O$50</c:f>
+              <c:f>'Final results'!$O$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10338,7 +10338,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$51:$I$56</c:f>
+              <c:f>'Final results'!$I$51:$I$56</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10364,7 +10364,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$O$51:$O$56</c:f>
+              <c:f>'Final results'!$O$51:$O$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10685,7 +10685,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$B$75</c:f>
+              <c:f>'Final results'!$B$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10706,7 +10706,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$76:$A$81</c:f>
+              <c:f>'Final results'!$A$76:$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10732,7 +10732,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$B$76:$B$81</c:f>
+              <c:f>'Final results'!$B$76:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10768,7 +10768,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$C$75</c:f>
+              <c:f>'Final results'!$C$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10789,7 +10789,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$76:$A$81</c:f>
+              <c:f>'Final results'!$A$76:$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10815,7 +10815,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$C$76:$C$81</c:f>
+              <c:f>'Final results'!$C$76:$C$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10851,7 +10851,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$D$75</c:f>
+              <c:f>'Final results'!$D$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10872,7 +10872,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$76:$A$81</c:f>
+              <c:f>'Final results'!$A$76:$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10898,7 +10898,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$D$76:$D$81</c:f>
+              <c:f>'Final results'!$D$76:$D$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10934,7 +10934,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$E$75</c:f>
+              <c:f>'Final results'!$E$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10955,7 +10955,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$76:$A$81</c:f>
+              <c:f>'Final results'!$A$76:$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -10981,7 +10981,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$E$76:$E$81</c:f>
+              <c:f>'Final results'!$E$76:$E$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11017,7 +11017,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$F$75</c:f>
+              <c:f>'Final results'!$F$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11038,7 +11038,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$76:$A$81</c:f>
+              <c:f>'Final results'!$A$76:$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11064,7 +11064,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$F$76:$F$81</c:f>
+              <c:f>'Final results'!$F$76:$F$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11100,7 +11100,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$G$75</c:f>
+              <c:f>'Final results'!$G$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11121,7 +11121,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$A$76:$A$81</c:f>
+              <c:f>'Final results'!$A$76:$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11147,7 +11147,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$G$76:$G$81</c:f>
+              <c:f>'Final results'!$G$76:$G$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11468,7 +11468,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$J$75</c:f>
+              <c:f>'Final results'!$J$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11489,7 +11489,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$76:$I$81</c:f>
+              <c:f>'Final results'!$I$76:$I$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11515,7 +11515,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$J$76:$J$81</c:f>
+              <c:f>'Final results'!$J$76:$J$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11551,7 +11551,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$K$75</c:f>
+              <c:f>'Final results'!$K$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11572,7 +11572,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$76:$I$81</c:f>
+              <c:f>'Final results'!$I$76:$I$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11598,7 +11598,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$K$76:$K$81</c:f>
+              <c:f>'Final results'!$K$76:$K$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11634,7 +11634,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$L$75</c:f>
+              <c:f>'Final results'!$L$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11655,7 +11655,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$76:$I$81</c:f>
+              <c:f>'Final results'!$I$76:$I$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11681,7 +11681,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$L$76:$L$81</c:f>
+              <c:f>'Final results'!$L$76:$L$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11717,7 +11717,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$M$75</c:f>
+              <c:f>'Final results'!$M$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11738,7 +11738,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$76:$I$81</c:f>
+              <c:f>'Final results'!$I$76:$I$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11764,7 +11764,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$M$76:$M$81</c:f>
+              <c:f>'Final results'!$M$76:$M$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11800,7 +11800,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$N$75</c:f>
+              <c:f>'Final results'!$N$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11821,7 +11821,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$76:$I$81</c:f>
+              <c:f>'Final results'!$I$76:$I$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11847,7 +11847,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$N$76:$N$81</c:f>
+              <c:f>'Final results'!$N$76:$N$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11883,7 +11883,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Retry!$O$75</c:f>
+              <c:f>'Final results'!$O$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11904,7 +11904,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Retry!$I$76:$I$81</c:f>
+              <c:f>'Final results'!$I$76:$I$81</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -11930,7 +11930,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Retry!$O$76:$O$81</c:f>
+              <c:f>'Final results'!$O$76:$O$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -30210,9 +30210,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
+      <xdr:colOff>463176</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30347,16 +30347,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>455820</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>110297</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>1131129</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:rowOff>8697</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30420,15 +30420,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
+      <xdr:colOff>411645</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>23052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>894245</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>127827</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33844,8 +33844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7973F6-D3D5-4592-94A3-FCA0F73C3305}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P86" sqref="P86"/>
+    <sheetView tabSelected="1" topLeftCell="B79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -33854,7 +33854,7 @@
     <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.4140625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.08203125" customWidth="1"/>
     <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
feat:  add CompareWordsVsWords by using Word2Vec method
</commit_message>
<xml_diff>
--- a/Documentation/CosineSimilarity/Record.xlsx
+++ b/Documentation/CosineSimilarity/Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\embeders-semantic-analysis\Documentation\CosineSimilarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A71884A-50D0-4567-AAA2-1B69878E4C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899E149D-5FF2-4EF0-9B5E-231A9BB4A8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="4" activeTab="6" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="4" activeTab="7" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="words vs words (3-small)" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="words vs pdfs (ada-002)" sheetId="5" r:id="rId5"/>
     <sheet name="words vs datasets (ada-002)" sheetId="7" r:id="rId6"/>
     <sheet name="Final results" sheetId="9" r:id="rId7"/>
+    <sheet name="word2Vec" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="113">
   <si>
     <t>political</t>
   </si>
@@ -503,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -531,6 +532,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12077,6 +12079,782 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1446468688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Words vs Words (Word2Vec)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>word2Vec!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>government</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>political</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>economic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sociological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>technological</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>legal</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>environmental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>word2Vec!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.49532101099999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44626144899999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.4927711999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.166628149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41135462699999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35091778099999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E0F-4914-94A9-4F9A2EC86FAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>word2Vec!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>automation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>political</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>economic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sociological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>technological</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>legal</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>environmental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>word2Vec!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-8.8648902000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2045266000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.107210744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32021822599999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0816144999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.117910599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E0F-4914-94A9-4F9A2EC86FAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>word2Vec!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>export duty</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>political</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>economic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sociological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>technological</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>legal</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>environmental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>word2Vec!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.147921365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37718162500000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0892077E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20668536000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28581256399999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24809383800000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7E0F-4914-94A9-4F9A2EC86FAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>word2Vec!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>demographics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>political</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>economic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sociological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>technological</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>legal</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>environmental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>word2Vec!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.17401957800000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18832628000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25616615700000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18121828200000001</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>-5.4400000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6485467000000005E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7E0F-4914-94A9-4F9A2EC86FAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>word2Vec!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>copyright laws</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>political</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>economic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sociological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>technological</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>legal</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>environmental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>word2Vec!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.20479903399999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21141043200000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8515530000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20783763699999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56394345400000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36990352700000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7E0F-4914-94A9-4F9A2EC86FAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>word2Vec!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>renewable energy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>political</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>economic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sociological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>technological</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>legal</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>environmental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>word2Vec!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.16149650500000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33107563400000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2369801E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31764612199999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14807244</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.449528873</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7E0F-4914-94A9-4F9A2EC86FAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1433178016"/>
+        <c:axId val="1433176576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1433178016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1433176576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1433176576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1433178016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18275,6 +19053,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -25626,6 +26444,511 @@
 </file>
 
 <file path=xl/charts/style22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -30492,6 +31815,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A53440-11EB-7670-435A-3231CE295962}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -33844,7 +35208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7973F6-D3D5-4592-94A3-FCA0F73C3305}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
@@ -35029,4 +36393,182 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A70A27-215E-482F-9221-203A41A8040A}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>0.49532101099999998</v>
+      </c>
+      <c r="C2">
+        <v>0.44626144899999998</v>
+      </c>
+      <c r="D2">
+        <v>-5.4927711999999997E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.166628149</v>
+      </c>
+      <c r="F2">
+        <v>0.41135462699999997</v>
+      </c>
+      <c r="G2">
+        <v>0.35091778099999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3">
+        <v>-8.8648902000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>3.2045266000000003E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.107210744</v>
+      </c>
+      <c r="E3">
+        <v>0.32021822599999999</v>
+      </c>
+      <c r="F3">
+        <v>-4.0816144999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.117910599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4">
+        <v>0.147921365</v>
+      </c>
+      <c r="C4">
+        <v>0.37718162500000002</v>
+      </c>
+      <c r="D4">
+        <v>-1.0892077E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.20668536000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.28581256399999999</v>
+      </c>
+      <c r="G4">
+        <v>0.24809383800000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5">
+        <v>0.17401957800000001</v>
+      </c>
+      <c r="C5">
+        <v>0.18832628000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.25616615700000001</v>
+      </c>
+      <c r="E5">
+        <v>0.18121828200000001</v>
+      </c>
+      <c r="F5" s="11">
+        <v>-5.4400000000000001E-5</v>
+      </c>
+      <c r="G5">
+        <v>9.6485467000000005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6">
+        <v>0.20479903399999999</v>
+      </c>
+      <c r="C6">
+        <v>0.21141043200000001</v>
+      </c>
+      <c r="D6">
+        <v>4.8515530000000001E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.20783763699999999</v>
+      </c>
+      <c r="F6">
+        <v>0.56394345400000001</v>
+      </c>
+      <c r="G6">
+        <v>0.36990352700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>0.16149650500000001</v>
+      </c>
+      <c r="C7">
+        <v>0.33107563400000001</v>
+      </c>
+      <c r="D7">
+        <v>1.2369801E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.31764612199999998</v>
+      </c>
+      <c r="F7">
+        <v>0.14807244</v>
+      </c>
+      <c r="G7">
+        <v>0.449528873</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update the record file
</commit_message>
<xml_diff>
--- a/Documentation/CosineSimilarity/Record.xlsx
+++ b/Documentation/CosineSimilarity/Record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\embeders-semantic-analysis\Documentation\CosineSimilarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899E149D-5FF2-4EF0-9B5E-231A9BB4A8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DAF6B7-1943-4757-98BD-AD070CB98252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="4" activeTab="7" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="689" firstSheet="4" activeTab="6" xr2:uid="{0B6CED53-8839-4228-88B3-1E625FBF7FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="words vs words (3-small)" sheetId="1" r:id="rId1"/>
@@ -517,6 +517,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,7 +533,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12246,11 +12246,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>word2Vec!$A$2</c:f>
+              <c:f>word2Vec!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>government</c:v>
+                  <c:v>political</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12267,33 +12267,33 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:f>word2Vec!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>political</c:v>
+                  <c:v>government</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>economic</c:v>
+                  <c:v>automation</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>sociological</c:v>
+                  <c:v>export duty</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>technological</c:v>
+                  <c:v>demographics</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>legal</c:v>
+                  <c:v>copyright laws</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>environmental</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>word2Vec!$B$2:$G$2</c:f>
+              <c:f>word2Vec!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -12301,19 +12301,19 @@
                   <c:v>0.49532101099999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44626144899999998</c:v>
+                  <c:v>-8.8648902000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.4927711999999997E-2</c:v>
+                  <c:v>0.147921365</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.166628149</c:v>
+                  <c:v>0.17401957800000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41135462699999997</c:v>
+                  <c:v>0.20479903399999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35091778099999998</c:v>
+                  <c:v>0.16149650500000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12329,11 +12329,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>word2Vec!$A$3</c:f>
+              <c:f>word2Vec!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>automation</c:v>
+                  <c:v>economic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12350,53 +12350,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:f>word2Vec!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>political</c:v>
+                  <c:v>government</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>economic</c:v>
+                  <c:v>automation</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>sociological</c:v>
+                  <c:v>export duty</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>technological</c:v>
+                  <c:v>demographics</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>legal</c:v>
+                  <c:v>copyright laws</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>environmental</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>word2Vec!$B$3:$G$3</c:f>
+              <c:f>word2Vec!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-8.8648902000000002E-2</c:v>
+                  <c:v>0.44626144899999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.2045266000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.107210744</c:v>
+                  <c:v>0.37718162500000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32021822599999999</c:v>
+                  <c:v>0.18832628000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.0816144999999998E-2</c:v>
+                  <c:v>0.21141043200000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.117910599</c:v>
+                  <c:v>0.33107563400000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12412,11 +12412,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>word2Vec!$A$4</c:f>
+              <c:f>word2Vec!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>export duty</c:v>
+                  <c:v>sociological</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12433,53 +12433,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:f>word2Vec!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>political</c:v>
+                  <c:v>government</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>economic</c:v>
+                  <c:v>automation</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>sociological</c:v>
+                  <c:v>export duty</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>technological</c:v>
+                  <c:v>demographics</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>legal</c:v>
+                  <c:v>copyright laws</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>environmental</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>word2Vec!$B$4:$G$4</c:f>
+              <c:f>word2Vec!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.147921365</c:v>
+                  <c:v>-5.4927711999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37718162500000002</c:v>
+                  <c:v>0.107210744</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-1.0892077E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20668536000000001</c:v>
+                  <c:v>0.25616615700000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28581256399999999</c:v>
+                  <c:v>4.8515530000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24809383800000001</c:v>
+                  <c:v>1.2369801E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12495,11 +12495,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>word2Vec!$A$5</c:f>
+              <c:f>word2Vec!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>demographics</c:v>
+                  <c:v>technological</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12516,53 +12516,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:f>word2Vec!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>political</c:v>
+                  <c:v>government</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>economic</c:v>
+                  <c:v>automation</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>sociological</c:v>
+                  <c:v>export duty</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>technological</c:v>
+                  <c:v>demographics</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>legal</c:v>
+                  <c:v>copyright laws</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>environmental</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>word2Vec!$B$5:$G$5</c:f>
+              <c:f>word2Vec!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.17401957800000001</c:v>
+                  <c:v>0.166628149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18832628000000001</c:v>
+                  <c:v>0.32021822599999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25616615700000001</c:v>
+                  <c:v>0.20668536000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.18121828200000001</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>-5.4400000000000001E-5</c:v>
+                <c:pt idx="4">
+                  <c:v>0.20783763699999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6485467000000005E-2</c:v>
+                  <c:v>0.31764612199999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12578,11 +12578,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>word2Vec!$A$6</c:f>
+              <c:f>word2Vec!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>copyright laws</c:v>
+                  <c:v>legal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12599,53 +12599,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:f>word2Vec!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>political</c:v>
+                  <c:v>government</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>economic</c:v>
+                  <c:v>automation</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>sociological</c:v>
+                  <c:v>export duty</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>technological</c:v>
+                  <c:v>demographics</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>legal</c:v>
+                  <c:v>copyright laws</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>environmental</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>word2Vec!$B$6:$G$6</c:f>
+              <c:f>word2Vec!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.20479903399999999</c:v>
+                  <c:v>0.41135462699999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21141043200000001</c:v>
+                  <c:v>-4.0816144999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8515530000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.20783763699999999</c:v>
+                  <c:v>0.28581256399999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>-5.4400000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.56394345400000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36990352700000001</c:v>
+                  <c:v>0.14807244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12661,11 +12661,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>word2Vec!$A$7</c:f>
+              <c:f>word2Vec!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>renewable energy</c:v>
+                  <c:v>environmental</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12682,50 +12682,50 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>word2Vec!$B$1:$G$1</c:f>
+              <c:f>word2Vec!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>political</c:v>
+                  <c:v>government</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>economic</c:v>
+                  <c:v>automation</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>sociological</c:v>
+                  <c:v>export duty</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>technological</c:v>
+                  <c:v>demographics</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>legal</c:v>
+                  <c:v>copyright laws</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>environmental</c:v>
+                  <c:v>renewable energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>word2Vec!$B$7:$G$7</c:f>
+              <c:f>word2Vec!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.16149650500000001</c:v>
+                  <c:v>0.35091778099999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33107563400000001</c:v>
+                  <c:v>0.117910599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2369801E-2</c:v>
+                  <c:v>0.24809383800000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31764612199999998</c:v>
+                  <c:v>9.6485467000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14807244</c:v>
+                  <c:v>0.36990352700000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.449528873</c:v>
@@ -12806,6 +12806,7 @@
         <c:axId val="1433176576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -31826,7 +31827,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:colOff>577850</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>149225</xdr:rowOff>
     </xdr:to>
@@ -32188,14 +32189,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
@@ -32356,14 +32357,14 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
@@ -32547,19 +32548,19 @@
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11">
       <c r="B37" t="s">
@@ -32971,14 +32972,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
@@ -33258,15 +33259,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
@@ -33474,15 +33475,15 @@
     </row>
     <row r="17" spans="1:7" ht="14.5" thickBot="1"/>
     <row r="18" spans="1:7" ht="14.5" thickBot="1">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="14.5" thickBot="1">
       <c r="A19" s="2"/>
@@ -33645,15 +33646,15 @@
     </row>
     <row r="35" spans="1:16" ht="14.5" thickBot="1"/>
     <row r="36" spans="1:16" ht="14.5" customHeight="1" thickBot="1">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:16">
       <c r="B37" t="s">
@@ -33850,15 +33851,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -35208,7 +35209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7973F6-D3D5-4592-94A3-FCA0F73C3305}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView topLeftCell="B88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
@@ -36399,13 +36400,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A70A27-215E-482F-9221-203A41A8040A}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36514,7 +36516,7 @@
       <c r="E5">
         <v>0.18121828200000001</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="6">
         <v>-5.4400000000000001E-5</v>
       </c>
       <c r="G5">

</xml_diff>